<commit_message>
Minor updates after review
Corrected minor errors after having the documentation reviewed.
Added CAD files in STEP and Fusion 360 formats.
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Light_Touch_Switch_BOM.xlsx
+++ b/Documentation/Working_Documents/Light_Touch_Switch_BOM.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc-my.sharepoint.com/personal/stephand_neilsquire_ca/Documents/Documents/GitHub/Light-Touch-Switch/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="472" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA32F918-D527-4744-BEE3-B738CA64B83A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50701356-55AA-4602-B8D6-E0FFE5BA90F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM" sheetId="2" r:id="rId1"/>
+    <sheet name="Light_Touch_Switch_BOM" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
   <si>
     <t>Total filament (g)</t>
   </si>
@@ -247,6 +247,36 @@
   </si>
   <si>
     <t>T01</t>
+  </si>
+  <si>
+    <t>Needle Nosed Pliers</t>
+  </si>
+  <si>
+    <t>Switch Testing Device</t>
+  </si>
+  <si>
+    <t>T02</t>
+  </si>
+  <si>
+    <t>T03</t>
+  </si>
+  <si>
+    <t>T04</t>
+  </si>
+  <si>
+    <t>T05</t>
+  </si>
+  <si>
+    <t>T06</t>
+  </si>
+  <si>
+    <t>T07</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/tensility-international-corp/10-00344/2350247</t>
+  </si>
+  <si>
+    <t>Tensility International Corp</t>
   </si>
 </sst>
 </file>
@@ -257,7 +287,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +339,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -585,7 +621,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -654,9 +690,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="13" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
@@ -953,7 +991,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,17 +1016,17 @@
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1033,11 +1071,11 @@
       <c r="J5" s="47"/>
       <c r="K5" s="48">
         <f>K6+K14</f>
-        <v>2.3650000000000002</v>
+        <v>5.89</v>
       </c>
       <c r="L5" s="49">
         <f>L6+L14</f>
-        <v>3.7100000000000004</v>
+        <v>5.89</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1057,11 +1095,11 @@
       <c r="J6" s="6"/>
       <c r="K6" s="52">
         <f>SUM(K8:K13)</f>
-        <v>2.165</v>
+        <v>5.6899999999999995</v>
       </c>
       <c r="L6" s="7">
-        <f>SUM(L8:L14)</f>
-        <v>3.5100000000000002</v>
+        <f>SUM(L8:L13)</f>
+        <v>5.6899999999999995</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -1159,13 +1197,13 @@
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G9" s="14">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="14">
         <v>1</v>
@@ -1175,19 +1213,19 @@
         <v>1</v>
       </c>
       <c r="J9" s="9">
-        <v>2.29</v>
+        <v>4.67</v>
       </c>
       <c r="K9" s="9">
         <f t="shared" si="1"/>
-        <v>1.145</v>
+        <v>4.67</v>
       </c>
       <c r="L9" s="9">
         <f t="shared" ref="L9:L12" si="2">I9*J9</f>
-        <v>2.29</v>
+        <v>4.67</v>
       </c>
       <c r="M9" s="14"/>
-      <c r="N9" s="14" t="s">
-        <v>54</v>
+      <c r="N9" s="66" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1472,7 +1510,9 @@
       <c r="N18" s="15"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="15" t="s">
+        <v>76</v>
+      </c>
       <c r="B19" s="15" t="s">
         <v>62</v>
       </c>
@@ -1582,9 +1622,11 @@
       <c r="N23" s="22"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="B24" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
@@ -1600,7 +1642,9 @@
       <c r="N24" s="16"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="22" t="s">
+        <v>73</v>
+      </c>
       <c r="B25" s="16" t="s">
         <v>42</v>
       </c>
@@ -1618,9 +1662,11 @@
       <c r="N25" s="16"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="B26" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -1636,8 +1682,12 @@
       <c r="N26" s="16"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="64" t="s">
+        <v>70</v>
+      </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1652,8 +1702,12 @@
       <c r="N27" s="16"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
+      <c r="A28" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>71</v>
+      </c>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
@@ -1807,20 +1861,22 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="105" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>65</v>
+      </c>
       <c r="B33" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="63" t="s">
-        <v>60</v>
+        <v>51</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17" t="s">
         <v>52</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G33" s="17">
         <v>0.5</v>
@@ -1831,37 +1887,61 @@
       <c r="I33" s="17">
         <v>1</v>
       </c>
-      <c r="J33" s="61">
-        <v>1.99</v>
-      </c>
-      <c r="K33" s="60">
-        <f>IF(G33&gt;0,J33/H33*G33,0)</f>
-        <v>0.995</v>
-      </c>
-      <c r="L33" s="60">
-        <f>J33*I33</f>
-        <v>1.99</v>
+      <c r="J33" s="17">
+        <v>2.29</v>
+      </c>
+      <c r="K33" s="17">
+        <v>1.145</v>
+      </c>
+      <c r="L33" s="17">
+        <v>2.29</v>
       </c>
       <c r="M33" s="17"/>
       <c r="N33" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="H34" s="17">
+        <v>1</v>
+      </c>
+      <c r="I34" s="17">
+        <v>1</v>
+      </c>
+      <c r="J34" s="61">
+        <v>1.99</v>
+      </c>
+      <c r="K34" s="60">
+        <f>IF(G34&gt;0,J34/H34*G34,0)</f>
+        <v>0.995</v>
+      </c>
+      <c r="L34" s="60">
+        <f>J34*I34</f>
+        <v>1.99</v>
+      </c>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
@@ -1979,15 +2059,37 @@
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N8" r:id="rId1" xr:uid="{1128DE05-AFA4-48F6-A643-65E8D3E7F524}"/>
+    <hyperlink ref="N9" r:id="rId2" xr:uid="{AABB4FC6-EDD7-48DB-86C0-CEED11E71CE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B51EC7ECFAC78D4E8EF6CBAFFF0B3505" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c16a8de1b3ad07fcfe40131daee80152">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xmlns:ns3="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85720a748046338a72a4f25fe522aa39" ns2:_="" ns3:_="">
     <xsd:import namespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
@@ -2236,27 +2338,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E754FF-A61B-4A88-B516-AC8192A9AA35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2273,23 +2374,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
-    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>